<commit_message>
added excel files containing graphs, updated some existing graphs, and added a new test script
</commit_message>
<xml_diff>
--- a/results/03-17 results 1/regexpResults.xlsx
+++ b/results/03-17 results 1/regexpResults.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="regexpResults" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -27,9 +27,6 @@
     <t>Node Bandwidth</t>
   </si>
   <si>
-    <t>Node Concurrent Mean</t>
-  </si>
-  <si>
     <t>Node Mean</t>
   </si>
   <si>
@@ -39,13 +36,16 @@
     <t>PHP Bandwidth</t>
   </si>
   <si>
-    <t>PHP Concurrent Mean</t>
-  </si>
-  <si>
     <t>PHP Mean</t>
   </si>
   <si>
     <t>PHP Longest</t>
+  </si>
+  <si>
+    <t>Node.js</t>
+  </si>
+  <si>
+    <t>Apache/PHP</t>
   </si>
 </sst>
 </file>
@@ -610,21 +610,21 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Bandwidth</a:t>
+              <a:rPr lang="en-US" sz="1200"/>
+              <a:t>Bandwidth for string search</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -643,16 +643,16 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -834,11 +834,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="399849368"/>
-        <c:axId val="399853288"/>
+        <c:axId val="397549312"/>
+        <c:axId val="397546568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="399849368"/>
+        <c:axId val="397549312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -858,20 +858,15 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Concurrency</a:t>
+                  <a:t>Concurrency (maximum simultaneous requests)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> (maximum simultaneous requests)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -896,9 +891,9 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="en-US"/>
@@ -934,15 +929,15 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="399853288"/>
+        <c:crossAx val="397546568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -950,7 +945,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="399853288"/>
+        <c:axId val="397546568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -984,20 +979,15 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Requests</a:t>
+                  <a:t>Requests per second</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> per second</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1022,9 +1012,9 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="en-US"/>
@@ -1054,15 +1044,15 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="399849368"/>
+        <c:crossAx val="397549312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1097,9 +1087,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -1130,7 +1120,10 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -1164,36 +1157,22 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Mean</a:t>
+              <a:rPr lang="en-US" sz="1200"/>
+              <a:t>Mean time-to-add for string search</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> time per request</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t>over all concurrent requests</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1211,16 +1190,16 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -1243,7 +1222,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Node Concurrent Mean</c:v>
+                  <c:v>Node.js</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1322,7 +1301,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PHP Concurrent Mean</c:v>
+                  <c:v>Apache/PHP</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1402,11 +1381,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="411485232"/>
-        <c:axId val="411482488"/>
+        <c:axId val="397537160"/>
+        <c:axId val="397539512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="411485232"/>
+        <c:axId val="397537160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1426,20 +1405,15 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Concurrency (maximum simultaneous</a:t>
+                  <a:t>Concurrency level</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> requests)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1464,9 +1438,9 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="en-US"/>
@@ -1502,15 +1476,15 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="411482488"/>
+        <c:crossAx val="397539512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1518,7 +1492,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="411482488"/>
+        <c:axId val="397539512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1552,9 +1526,9 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
@@ -1585,9 +1559,9 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="en-US"/>
@@ -1617,15 +1591,15 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="411485232"/>
+        <c:crossAx val="397537160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1660,9 +1634,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -1693,7 +1667,10 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -1727,27 +1704,22 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Mean versus</a:t>
+              <a:rPr lang="en-US" sz="1200"/>
+              <a:t>Mean versus longest for string search</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> longest</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1765,16 +1737,16 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -1789,7 +1761,7 @@
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>regexpResults!$D$1</c:f>
@@ -1872,7 +1844,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
               <c:f>regexpResults!$E$1</c:f>
@@ -1955,7 +1927,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="6"/>
           <c:tx>
             <c:strRef>
               <c:f>regexpResults!$H$1</c:f>
@@ -2037,7 +2009,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:order val="7"/>
           <c:tx>
             <c:strRef>
               <c:f>regexpResults!$I$1</c:f>
@@ -2126,11 +2098,429 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="399837608"/>
-        <c:axId val="399843488"/>
+        <c:axId val="397543824"/>
+        <c:axId val="397546176"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>regexpResults!$D$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Node Mean</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent5"/>
+                    </a:solidFill>
+                    <a:prstDash val="dash"/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>regexpResults!$A$2:$A$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>64</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>regexpResults!$D$2:$D$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>1559.6125999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>3116.3002000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>6241.1809999999996</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>12476.902</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>24931.963399999899</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>50007.4471999999</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="5"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>regexpResults!$E$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Node Longest</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6"/>
+                    </a:solidFill>
+                    <a:prstDash val="sysDot"/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>regexpResults!$A$2:$A$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>64</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>regexpResults!$E$2:$E$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>1728.6</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>3176.4</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>6296.2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>12523.8</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>24956.799999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>49823.199999999997</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="6"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>regexpResults!$H$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>PHP Mean</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>regexpResults!$A$2:$A$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>64</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>regexpResults!$H$2:$H$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>7560.0781999999899</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>14908.946</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>29401.371200000001</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>57215.4398</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>112673.8774</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>226340.79479999901</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="7"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>regexpResults!$I$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>PHP Longest</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2">
+                        <a:lumMod val="60000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>regexpResults!$A$2:$A$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>64</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>regexpResults!$I$2:$I$7</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>7928</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>15506.4</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>30360.799999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>60016.6</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>119395.4</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>226184.8</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="399837608"/>
+        <c:axId val="397543824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2150,9 +2540,9 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
@@ -2183,9 +2573,9 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="en-US"/>
@@ -2221,15 +2611,15 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="399843488"/>
+        <c:crossAx val="397546176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2237,7 +2627,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="399843488"/>
+        <c:axId val="397546176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2271,9 +2661,9 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
@@ -2304,9 +2694,9 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="en-US"/>
@@ -2336,15 +2726,15 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="399837608"/>
+        <c:crossAx val="397543824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2379,9 +2769,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -2412,7 +2802,750 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200"/>
+              <a:t>String search</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="0"/>
+              <a:t> m</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200"/>
+              <a:t>ean versus longest</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200"/>
+              <a:t>(with logarithmic</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="0"/>
+              <a:t> y-axis)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1200"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>regexpResults!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Node Mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>regexpResults!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>regexpResults!$D$2:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1559.6125999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3116.3002000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6241.1809999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12476.902</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24931.963399999899</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50007.4471999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>regexpResults!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Node Longest</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>regexpResults!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>regexpResults!$E$2:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1728.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3176.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6296.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12523.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24956.799999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>49823.199999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>regexpResults!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PHP Mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>regexpResults!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>regexpResults!$H$2:$H$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>7560.0781999999899</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14908.946</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29401.371200000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>57215.4398</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>112673.8774</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>226340.79479999901</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>regexpResults!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PHP Longest</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>regexpResults!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>regexpResults!$I$2:$I$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>7928</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15506.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30360.799999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60016.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>119395.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>226184.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="397539904"/>
+        <c:axId val="397552056"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="397539904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Concurrency (maximum simultaneous requests)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="397552056"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="397552056"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Millilseconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="397539904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -2545,6 +3678,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3552,6 +4725,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4139,8 +5828,8 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>566737</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4154,6 +5843,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4425,10 +6146,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="I1" activeCellId="3" sqref="D1:D1048576 E1:E1048576 H1:H1048576 I1:I1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4444,7 +6165,7 @@
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4452,28 +6173,28 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -4502,7 +6223,7 @@
         <v>7928</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
@@ -4531,7 +6252,7 @@
         <v>15506.4</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>8</v>
       </c>
@@ -4560,7 +6281,7 @@
         <v>30360.799999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>16</v>
       </c>
@@ -4589,7 +6310,7 @@
         <v>60016.6</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>32</v>
       </c>
@@ -4618,7 +6339,7 @@
         <v>119395.4</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>64</v>
       </c>
@@ -4646,6 +6367,10 @@
       <c r="I7">
         <v>226184.8</v>
       </c>
+      <c r="J7">
+        <f>(I7/H7)</f>
+        <v>0.99931079680029899</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>